<commit_message>
Added code for 200 OK
Added code for 200 OK
</commit_message>
<xml_diff>
--- a/src/com/amex/testdata/API_Details.xlsx
+++ b/src/com/amex/testdata/API_Details.xlsx
@@ -441,9 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -543,7 +541,7 @@
         <v>13</v>
       </c>
       <c r="H3">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Request and Response is stored in files
</commit_message>
<xml_diff>
--- a/src/com/amex/testdata/API_Details.xlsx
+++ b/src/com/amex/testdata/API_Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
   <si>
     <t>Request_Name</t>
   </si>
@@ -146,7 +146,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,19 +494,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1"/>
-    <col min="3" max="3" width="40.28515625" bestFit="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.140625" bestFit="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1"/>
-    <col min="8" max="8" width="22.7109375"/>
-    <col min="9" max="9" width="25.7109375" bestFit="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1"/>
-    <col min="11" max="11" width="23.5703125"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" hidden="false" bestFit="false" style="0"/>
+    <col min="2" max="2" width="11.28515625" hidden="false" bestFit="true" style="0"/>
+    <col min="3" max="3" width="40.28515625" hidden="false" bestFit="true" style="0"/>
+    <col min="4" max="4" width="16.42578125" hidden="false" bestFit="true" style="0"/>
+    <col min="5" max="5" width="15.0" hidden="false" bestFit="true" style="0"/>
+    <col min="6" max="6" width="34.140625" hidden="false" bestFit="true" style="0"/>
+    <col min="7" max="7" width="18.7109375" hidden="false" bestFit="true" style="0"/>
+    <col min="8" max="8" width="22.7109375" hidden="false" bestFit="false" style="0"/>
+    <col min="9" max="9" width="25.7109375" hidden="false" bestFit="true" style="0"/>
+    <col min="10" max="10" width="16.5703125" hidden="false" bestFit="true" style="0"/>
+    <col min="11" max="11" width="23.5703125" hidden="false" bestFit="false" style="0"/>
+    <col min="12" max="12" width="11.42890625" hidden="false" bestFit="true" style="0" customWidth="true"/>
+    <col min="13" max="13" width="13.378515625" hidden="false" bestFit="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Merging phase1 to trunk
</commit_message>
<xml_diff>
--- a/src/com/amex/testdata/API_Details.xlsx
+++ b/src/com/amex/testdata/API_Details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="13395" windowHeight="5130"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="13395" windowHeight="5070"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
   <si>
     <t>Request_Name</t>
   </si>
@@ -111,12 +111,43 @@
   <si>
     <t>TC_003</t>
   </si>
+  <si>
+    <t>Run_Mode</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Test_Result</t>
+  </si>
+  <si>
+    <t>Failure_Cause</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Exp response: 401 Act response: 400</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,13 +176,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,141 +488,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" hidden="false" bestFit="false" style="0"/>
+    <col min="2" max="2" width="11.28515625" hidden="false" bestFit="true" style="0"/>
+    <col min="3" max="3" width="40.28515625" hidden="false" bestFit="true" style="0"/>
+    <col min="4" max="4" width="16.42578125" hidden="false" bestFit="true" style="0"/>
+    <col min="5" max="5" width="15.0" hidden="false" bestFit="true" style="0"/>
+    <col min="6" max="6" width="34.140625" hidden="false" bestFit="true" style="0"/>
+    <col min="7" max="7" width="18.7109375" hidden="false" bestFit="true" style="0"/>
+    <col min="8" max="8" width="22.7109375" hidden="false" bestFit="false" style="0"/>
+    <col min="9" max="9" width="25.7109375" hidden="false" bestFit="true" style="0"/>
+    <col min="10" max="10" width="16.5703125" hidden="false" bestFit="true" style="0"/>
+    <col min="11" max="11" width="23.5703125" hidden="false" bestFit="false" style="0"/>
+    <col min="12" max="12" width="11.42890625" hidden="false" bestFit="true" style="0" customWidth="true"/>
+    <col min="13" max="13" width="13.378515625" hidden="false" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2">
+      <c r="I2" s="3">
         <v>200</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3">
-        <v>400</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3">
+        <v>401</v>
+      </c>
+      <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="3">
         <v>200</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>